<commit_message>
this is updated database
</commit_message>
<xml_diff>
--- a/Uniform_inventory_ccf.xlsx
+++ b/Uniform_inventory_ccf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushpndya/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B96AB9E-A46E-A54C-BA49-F670830343BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E72E93E-FA08-DB4A-A248-A8CE765D9127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D325EE59-E00C-42FA-ACA3-560EA915EB94}"/>
+    <workbookView xWindow="1020" yWindow="660" windowWidth="13940" windowHeight="15860" xr2:uid="{D325EE59-E00C-42FA-ACA3-560EA915EB94}"/>
   </bookViews>
   <sheets>
     <sheet name="No. 3s" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="154">
   <si>
     <t>Shirts</t>
   </si>
@@ -52,15 +52,9 @@
     <t>Jumpers</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -497,6 +491,18 @@
   </si>
   <si>
     <t>WO1C</t>
+  </si>
+  <si>
+    <t>Male Shirts</t>
+  </si>
+  <si>
+    <t>Female Shirts</t>
+  </si>
+  <si>
+    <t>Male Trousers</t>
+  </si>
+  <si>
+    <t>Female Trousers</t>
   </si>
 </sst>
 </file>
@@ -863,316 +869,307 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M3">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M4">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M5">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M8">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M9">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10">
-        <v>118</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
         <v>53</v>
@@ -1182,9 +1179,6 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>48</v>
-      </c>
       <c r="G19" t="s">
         <v>55</v>
       </c>
@@ -1212,161 +1206,148 @@
       <c r="G22" t="s">
         <v>61</v>
       </c>
-      <c r="J22" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:N1"/>
-  </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -1398,119 +1379,119 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2">
         <v>82</v>
       </c>
       <c r="J2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3">
         <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5">
         <v>102</v>
       </c>
       <c r="J5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6">
         <v>108</v>
       </c>
       <c r="J6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7">
         <v>112</v>
@@ -1518,176 +1499,176 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1716,100 +1697,100 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1838,36 +1819,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2048,55 +2029,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2125,40 +2106,40 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
omg I had to reupload file nooo
</commit_message>
<xml_diff>
--- a/Uniform_inventory_ccf.xlsx
+++ b/Uniform_inventory_ccf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushpndya/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E72E93E-FA08-DB4A-A248-A8CE765D9127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9BDB874-2BAF-B240-8BA5-CFE83AC38150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="660" windowWidth="13940" windowHeight="15860" xr2:uid="{D325EE59-E00C-42FA-ACA3-560EA915EB94}"/>
+    <workbookView xWindow="5840" yWindow="720" windowWidth="13940" windowHeight="15860" xr2:uid="{D325EE59-E00C-42FA-ACA3-560EA915EB94}"/>
   </bookViews>
   <sheets>
     <sheet name="No. 3s" sheetId="3" r:id="rId1"/>

</xml_diff>